<commit_message>
[afin-dev] Starting implementing TestRepoSetup (in conway.test)
</commit_message>
<xml_diff>
--- a/8001/EXPECTED@latest/Operator Reports/DevOps/Repo Stats.xlsx
+++ b/8001/EXPECTED@latest/Operator Reports/DevOps/Repo Stats.xlsx
@@ -1,31 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alex\Code\conway_fork\conway.scenarios\8001\EXPECTED@latest\Operator Reports\DevOps\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9631D-686A-4B4F-AE14-D331232DCD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="foo_app.svc (Local)" sheetId="2" r:id="rId2"/>
-    <sheet name="foo_app.svc (Remote)" sheetId="3" r:id="rId3"/>
-    <sheet name="foo_app.docs (Local)" sheetId="4" r:id="rId4"/>
-    <sheet name="foo_app.docs (Remote)" sheetId="5" r:id="rId5"/>
-    <sheet name="foo_app.test (Local)" sheetId="6" r:id="rId6"/>
-    <sheet name="foo_app.test (Remote)" sheetId="7" r:id="rId7"/>
-    <sheet name="foo_app.scenarios (Local)" sheetId="8" r:id="rId8"/>
-    <sheet name="foo_app.scenarios (Remote)" sheetId="9" r:id="rId9"/>
-    <sheet name="foo_app.ops (Local)" sheetId="10" r:id="rId10"/>
-    <sheet name="foo_app.ops (Remote)" sheetId="11" r:id="rId11"/>
+    <sheet name="foo_app.docs (Local)" sheetId="2" r:id="rId2"/>
+    <sheet name="foo_app.docs (Remote)" sheetId="3" r:id="rId3"/>
+    <sheet name="foo_app.ops (Local)" sheetId="4" r:id="rId4"/>
+    <sheet name="foo_app.ops (Remote)" sheetId="5" r:id="rId5"/>
+    <sheet name="foo_app.scenarios (Local)" sheetId="6" r:id="rId6"/>
+    <sheet name="foo_app.scenarios (Remote)" sheetId="7" r:id="rId7"/>
+    <sheet name="foo_app.svc (Local)" sheetId="8" r:id="rId8"/>
+    <sheet name="foo_app.svc (Remote)" sheetId="9" r:id="rId9"/>
+    <sheet name="foo_app.test (Local)" sheetId="10" r:id="rId10"/>
+    <sheet name="foo_app.test (Remote)" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -44,6 +38,12 @@
     <t># Untracked files</t>
   </si>
   <si>
+    <t># Modified files</t>
+  </si>
+  <si>
+    <t># Deleted files</t>
+  </si>
+  <si>
     <t>Last commit</t>
   </si>
   <si>
@@ -53,6 +53,9 @@
     <t>Last commit hash</t>
   </si>
   <si>
+    <t>foo_app.docs</t>
+  </si>
+  <si>
     <t>Local</t>
   </si>
   <si>
@@ -68,6 +71,21 @@
     <t>Remote</t>
   </si>
   <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>foo_app.ops</t>
+  </si>
+  <si>
+    <t>foo_app.scenarios</t>
+  </si>
+  <si>
+    <t>foo_app.svc</t>
+  </si>
+  <si>
+    <t>foo_app.test</t>
+  </si>
+  <si>
     <t>Commit #</t>
   </si>
   <si>
@@ -93,37 +111,13 @@
   </si>
   <si>
     <t>README.md</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t># Modified files</t>
-  </si>
-  <si>
-    <t># Deleted files</t>
-  </si>
-  <si>
-    <t>foo_app.svc</t>
-  </si>
-  <si>
-    <t>foo_app.docs</t>
-  </si>
-  <si>
-    <t>foo_app.test</t>
-  </si>
-  <si>
-    <t>foo_app.scenarios</t>
-  </si>
-  <si>
-    <t>foo_app.ops</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,14 +198,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -258,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,27 +276,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,24 +310,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -535,27 +485,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
-    <col min="9" max="9" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,30 +519,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -604,228 +554,228 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
@@ -836,24 +786,24 @@
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -865,13 +815,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -880,94 +830,94 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -976,94 +926,94 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1072,94 +1022,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1168,94 +1118,94 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1264,94 +1214,94 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1360,94 +1310,94 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1456,94 +1406,94 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1552,94 +1502,94 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1648,94 +1598,94 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1744,94 +1694,94 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>